<commit_message>
Componente MenuCompleto funcionando, faltan ultimar detalles de diseño, logica de negocio perfecta excepto cuando se elimina el ultimo plato de las tarjetas peqieñas no se refrescan las tarjetas y agregar modal con explicacion de uso del componente
</commit_message>
<xml_diff>
--- a/control funciones menucompleto.xlsx
+++ b/control funciones menucompleto.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade_\Desktop\Delivery app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F9C10-4201-4372-A22D-139553FECF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33993607-198F-415D-87D1-1A7A101A8A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{B50175D1-3EDE-4D77-9654-8E7F3090148C}"/>
   </bookViews>
   <sheets>
     <sheet name="Funciones menucompletocompon" sheetId="1" r:id="rId1"/>
     <sheet name="q hacer" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t xml:space="preserve">AGREGAR TARJETA </t>
   </si>
@@ -72,10 +73,58 @@
     <t>BOTON BORRAR REFRESCA LISTA???</t>
   </si>
   <si>
-    <t>Al borrar el ultimo plato de cualquier card pequeña, se ve el modal de la lista vacio, pasa porque esta programado para mostrar la lista, BUSCAR UNA FORMA PARA QUE NO SE MUESTRE EL MODAL O LISTA CUANDO LA LISTA ESTA VACIA</t>
-  </si>
-  <si>
     <t>INPUTS BOTON AGREGAR SE BORRAN?</t>
+  </si>
+  <si>
+    <t>POSTRES</t>
+  </si>
+  <si>
+    <t>fas fa-ice-cream</t>
+  </si>
+  <si>
+    <t>POLLOS</t>
+  </si>
+  <si>
+    <t>fas fa-drumstick-bite</t>
+  </si>
+  <si>
+    <t>GUARNICIONES</t>
+  </si>
+  <si>
+    <t>fas fa-carrot</t>
+  </si>
+  <si>
+    <t>PIZZAS</t>
+  </si>
+  <si>
+    <t>fas fa-pizza-slice</t>
+  </si>
+  <si>
+    <t>CARNES</t>
+  </si>
+  <si>
+    <t>fas fa-utensils</t>
+  </si>
+  <si>
+    <t>PRUEBA</t>
+  </si>
+  <si>
+    <t>fff</t>
+  </si>
+  <si>
+    <t>BEBIDAS</t>
+  </si>
+  <si>
+    <t>fas fa-glass-cheers</t>
+  </si>
+  <si>
+    <t>ver que cuando se elimina el ultimo plato de las tarjetas peqieñas no se refrescan las tarjetas hasta que se refresca la pgina</t>
+  </si>
+  <si>
+    <t>ver en la api que no acepten las tablas valores nulos desde el front</t>
+  </si>
+  <si>
+    <t>agregar modal con explicacion de uso del componente</t>
   </si>
 </sst>
 </file>
@@ -251,6 +300,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -260,52 +324,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,44 +681,44 @@
     <col min="3" max="3" width="4.265625" customWidth="1"/>
     <col min="4" max="5" width="11.46484375" customWidth="1"/>
     <col min="6" max="6" width="4.265625" customWidth="1"/>
-    <col min="9" max="9" width="1.73046875" style="8" customWidth="1"/>
-    <col min="18" max="18" width="1.73046875" style="8" customWidth="1"/>
-    <col min="27" max="27" width="1.73046875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="1.73046875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="1.73046875" style="3" customWidth="1"/>
+    <col min="27" max="27" width="1.73046875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="K1" s="3" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
+      <c r="K1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="5"/>
-      <c r="T1" s="3" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="12"/>
+      <c r="T1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="5"/>
-      <c r="AC1" s="3" t="s">
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="12"/>
+      <c r="AC1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="5"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="12"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B2" s="1"/>
@@ -686,58 +735,58 @@
       <c r="AI2" s="1"/>
     </row>
     <row r="3" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="22"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="J3" s="6" t="s">
+      <c r="H3" s="22"/>
+      <c r="J3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="7"/>
+      <c r="N3" s="22"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="7"/>
-      <c r="S3" s="6" t="s">
+      <c r="Q3" s="22"/>
+      <c r="S3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="7"/>
+      <c r="T3" s="22"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="7"/>
+      <c r="W3" s="22"/>
       <c r="X3" s="2"/>
-      <c r="Y3" s="6" t="s">
+      <c r="Y3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="7"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="11"/>
+      <c r="Z3" s="22"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="14"/>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="6" t="s">
+      <c r="AE3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="AF3" s="7"/>
+      <c r="AF3" s="22"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="11"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="14"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
@@ -754,119 +803,119 @@
       <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="D5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="G5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="J5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="18"/>
-      <c r="M5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="18"/>
-      <c r="P5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="18"/>
-      <c r="S5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T5" s="18"/>
-      <c r="V5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="W5" s="18"/>
-      <c r="Y5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z5" s="18"/>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="11"/>
-      <c r="AE5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF5" s="18"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="11"/>
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="D5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="G5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="J5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="M5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="P5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="S5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="8"/>
+      <c r="V5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W5" s="8"/>
+      <c r="Y5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="8"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="14"/>
+      <c r="AE5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF5" s="8"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="14"/>
     </row>
     <row r="8" spans="1:35" ht="8.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="10" spans="1:35" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="K10" s="3" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="K10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="5"/>
-      <c r="T10" s="3" t="s">
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="12"/>
+      <c r="T10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="5"/>
-      <c r="AC10" s="3" t="s">
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="12"/>
+      <c r="AC10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="4"/>
-      <c r="AF10" s="4"/>
-      <c r="AG10" s="4"/>
-      <c r="AH10" s="5"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="12"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="C11" s="1"/>
@@ -882,51 +931,51 @@
       <c r="AI11" s="1"/>
     </row>
     <row r="12" spans="1:35" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="2"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="J12" s="12" t="s">
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="J12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="13"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N12" s="13"/>
+      <c r="N12" s="16"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="12" t="s">
+      <c r="P12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="13"/>
-      <c r="S12" s="12" t="s">
+      <c r="Q12" s="16"/>
+      <c r="S12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="T12" s="13"/>
+      <c r="T12" s="16"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="12" t="s">
+      <c r="V12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="W12" s="13"/>
+      <c r="W12" s="16"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="12" t="s">
+      <c r="Y12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Z12" s="13"/>
-      <c r="AB12" s="10"/>
-      <c r="AC12" s="11"/>
+      <c r="Z12" s="16"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="14"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="12" t="s">
+      <c r="AE12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AF12" s="13"/>
+      <c r="AF12" s="16"/>
       <c r="AG12" s="2"/>
-      <c r="AH12" s="10"/>
-      <c r="AI12" s="11"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="14"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="C13" s="1"/>
@@ -942,211 +991,216 @@
       <c r="AI13" s="1"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="B14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="J14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="18"/>
-      <c r="M14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="18"/>
-      <c r="P14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="18"/>
-      <c r="S14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T14" s="18"/>
-      <c r="V14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="W14" s="18"/>
-      <c r="Y14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z14" s="18"/>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="11"/>
-      <c r="AE14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF14" s="18"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="11"/>
+      <c r="B14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="J14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="M14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="P14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="S14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="8"/>
+      <c r="V14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W14" s="8"/>
+      <c r="Y14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="8"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="14"/>
+      <c r="AE14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="8"/>
+      <c r="AH14" s="13"/>
+      <c r="AI14" s="14"/>
     </row>
     <row r="17" spans="1:35" ht="8.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="8"/>
-      <c r="AG17" s="8"/>
-      <c r="AH17" s="8"/>
-      <c r="AI17" s="8"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="19" spans="1:35" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="K19" s="3" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="K19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="5"/>
-      <c r="T19" s="3" t="s">
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="12"/>
+      <c r="T19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="5"/>
-      <c r="AC19" s="3" t="s">
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="12"/>
+      <c r="AC19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AD19" s="4"/>
-      <c r="AE19" s="4"/>
-      <c r="AF19" s="4"/>
-      <c r="AG19" s="4"/>
-      <c r="AH19" s="5"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="12"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="E20" s="1"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
       <c r="W20" s="1"/>
-      <c r="X20" s="16"/>
-      <c r="Y20" s="16"/>
       <c r="AF20" s="1"/>
-      <c r="AG20" s="16"/>
-      <c r="AH20" s="16"/>
     </row>
     <row r="21" spans="1:35" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="M21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="V21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="W21" s="13"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
-      <c r="AE21" s="10"/>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="23"/>
-      <c r="AH21" s="23"/>
+      <c r="D21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="M21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="V21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="W21" s="16"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="14"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
       <c r="W22" s="1"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
       <c r="AF22" s="1"/>
-      <c r="AG22" s="16"/>
-      <c r="AH22" s="16"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="D23" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="M23" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" s="18"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="V23" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="W23" s="18"/>
-      <c r="X23" s="22"/>
-      <c r="Y23" s="22"/>
-      <c r="AE23" s="10"/>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="22"/>
-      <c r="AH23" s="22"/>
+      <c r="D23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="M23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="8"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="V23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W23" s="8"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="14"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AC19:AH19"/>
-    <mergeCell ref="AE21:AF21"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K19:P19"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AH14:AI14"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="T19:Y19"/>
-    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K10:P10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="P14:Q14"/>
     <mergeCell ref="T10:Y10"/>
     <mergeCell ref="S12:T12"/>
     <mergeCell ref="V12:W12"/>
@@ -1155,49 +1209,28 @@
     <mergeCell ref="AB12:AC12"/>
     <mergeCell ref="AE12:AF12"/>
     <mergeCell ref="AH12:AI12"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AH14:AI14"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="T19:Y19"/>
+    <mergeCell ref="V21:W21"/>
     <mergeCell ref="S14:T14"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="K10:P10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="T1:Y1"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K19:P19"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AC19:AH19"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AG23:AH23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1206,20 +1239,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB88519-6E38-4716-808F-E8354FD906F4}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="19">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="5">
         <v>45133</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G11" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B69C7B3-E8BA-4B68-BD27-6FCF9A94D355}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="6">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="6">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="6">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
+        <v>58</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Home Component practicamente terminado, faltan bordes de listasy ultimar alguna cosita en la db
</commit_message>
<xml_diff>
--- a/control funciones menucompleto.xlsx
+++ b/control funciones menucompleto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade_\Desktop\Delivery app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33993607-198F-415D-87D1-1A7A101A8A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE7ABE9-5743-4D53-9E3E-A5C873438D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{B50175D1-3EDE-4D77-9654-8E7F3090148C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{B50175D1-3EDE-4D77-9654-8E7F3090148C}"/>
   </bookViews>
   <sheets>
     <sheet name="Funciones menucompletocompon" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t xml:space="preserve">AGREGAR TARJETA </t>
   </si>
@@ -76,48 +76,6 @@
     <t>INPUTS BOTON AGREGAR SE BORRAN?</t>
   </si>
   <si>
-    <t>POSTRES</t>
-  </si>
-  <si>
-    <t>fas fa-ice-cream</t>
-  </si>
-  <si>
-    <t>POLLOS</t>
-  </si>
-  <si>
-    <t>fas fa-drumstick-bite</t>
-  </si>
-  <si>
-    <t>GUARNICIONES</t>
-  </si>
-  <si>
-    <t>fas fa-carrot</t>
-  </si>
-  <si>
-    <t>PIZZAS</t>
-  </si>
-  <si>
-    <t>fas fa-pizza-slice</t>
-  </si>
-  <si>
-    <t>CARNES</t>
-  </si>
-  <si>
-    <t>fas fa-utensils</t>
-  </si>
-  <si>
-    <t>PRUEBA</t>
-  </si>
-  <si>
-    <t>fff</t>
-  </si>
-  <si>
-    <t>BEBIDAS</t>
-  </si>
-  <si>
-    <t>fas fa-glass-cheers</t>
-  </si>
-  <si>
     <t>ver que cuando se elimina el ultimo plato de las tarjetas peqieñas no se refrescan las tarjetas hasta que se refresca la pgina</t>
   </si>
   <si>
@@ -125,13 +83,151 @@
   </si>
   <si>
     <t>agregar modal con explicacion de uso del componente</t>
+  </si>
+  <si>
+    <t>agregar boton que muestre lista coppleta</t>
+  </si>
+  <si>
+    <t>agregar boton descarga lista completa platos en excel</t>
+  </si>
+  <si>
+    <t>agregar fondo y bordes</t>
+  </si>
+  <si>
+    <t>donde se ageguen iconos o colores, poner lista representativa arriba de ese modal</t>
+  </si>
+  <si>
+    <t>ver que los textos se justifiquen</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1624552184280-9e9631bbeee9?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=687&amp;q=80</t>
+  </si>
+  <si>
+    <t>COCA-COLA</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1550505095-81378a674395?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=1470&amp;q=80</t>
+  </si>
+  <si>
+    <t>AGUA</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1529692236671-f1f6cf9683ba?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=1470&amp;q=80</t>
+  </si>
+  <si>
+    <t>ASADO AL HORNO</t>
+  </si>
+  <si>
+    <t>https://thumbs.dreamstime.com/z/schnitzel-28139717.jpg?w=576</t>
+  </si>
+  <si>
+    <t>MILANESAS</t>
+  </si>
+  <si>
+    <t>https://thumbs.dreamstime.com/z/chuleta-milanesa-de-la-carne-vaca-empanada-con-el-lim%C3%B3n-y-cierre-u-las-patatas-fritas-113148293.jpg?w=992</t>
+  </si>
+  <si>
+    <t>SUPREMA</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1615557960916-5f4791effe9d?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=1374&amp;q=80</t>
+  </si>
+  <si>
+    <t>POLLO AL HORNO</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1540420773420-3366772f4999?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=684&amp;q=80</t>
+  </si>
+  <si>
+    <t>ENSALADA</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1598679253544-2c97992403ea?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=687&amp;q=80</t>
+  </si>
+  <si>
+    <t>PAPAS FRITAS</t>
+  </si>
+  <si>
+    <t>https://plus.unsplash.com/premium_photo-1661427159078-9d85039e99b8?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=1632&amp;q=80</t>
+  </si>
+  <si>
+    <t>HELADO</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1593416981196-995e60a44d4a?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=686&amp;q=80</t>
+  </si>
+  <si>
+    <t>FLAN</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1571066811602-716837d681de?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=536&amp;q=80</t>
+  </si>
+  <si>
+    <t>PIZZA CON HUEVO</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1589187151053-5ec8818e661b?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=687&amp;q=80</t>
+  </si>
+  <si>
+    <t>PIZZA RUCULA</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1628809643597-654efb99b214?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=685&amp;q=80</t>
+  </si>
+  <si>
+    <t>BUDIN DE PAN</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1504649346668-2cc86afaa2e1?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=1364&amp;q=80</t>
+  </si>
+  <si>
+    <t>PAMPLONA</t>
+  </si>
+  <si>
+    <t>https://plus.unsplash.com/premium_photo-1676313449501-8ed94e22a65b?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=687&amp;q=80</t>
+  </si>
+  <si>
+    <t>ENSALDA RUSA</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1574071318508-1cdbab80d002?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=1469&amp;q=80</t>
+  </si>
+  <si>
+    <t>PIZZA CANCHA</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1624772398061-bbfa87ec6b5a?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=687&amp;q=80</t>
+  </si>
+  <si>
+    <t>CHORIZO</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1566633806327-68e152aaf26d?ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D&amp;auto=format&amp;fit=crop&amp;w=1470&amp;q=80</t>
+  </si>
+  <si>
+    <t>CERVEZA</t>
+  </si>
+  <si>
+    <t>ver  cambiar nombre columna TipoPlato en excel por id_TipoPlato</t>
+  </si>
+  <si>
+    <t>ocultar input con id de lo que sea</t>
+  </si>
+  <si>
+    <t>que no se puedan repetir los tipos de platos en la db</t>
+  </si>
+  <si>
+    <t>HACER MODALES MAS GRANDES</t>
+  </si>
+  <si>
+    <t>poner cabeceras a las listas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +255,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -306,15 +415,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -322,6 +425,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -336,25 +451,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA668CC3-189C-49D9-8DCE-DD0C686ACD39}">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V23" sqref="V23:W23"/>
     </sheetView>
   </sheetViews>
@@ -735,58 +846,58 @@
       <c r="AI2" s="1"/>
     </row>
     <row r="3" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="22"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="J3" s="21" t="s">
+      <c r="H3" s="14"/>
+      <c r="J3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="22"/>
+      <c r="K3" s="14"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="22"/>
+      <c r="N3" s="14"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="22"/>
-      <c r="S3" s="21" t="s">
+      <c r="Q3" s="14"/>
+      <c r="S3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="22"/>
+      <c r="T3" s="14"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="22"/>
+      <c r="W3" s="14"/>
       <c r="X3" s="2"/>
-      <c r="Y3" s="21" t="s">
+      <c r="Y3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="22"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="18"/>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="21" t="s">
+      <c r="AE3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="AF3" s="22"/>
+      <c r="AF3" s="14"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="13"/>
-      <c r="AI3" s="14"/>
+      <c r="AH3" s="17"/>
+      <c r="AI3" s="18"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
@@ -803,50 +914,50 @@
       <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="D5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="G5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="J5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="M5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="8"/>
-      <c r="P5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="8"/>
-      <c r="S5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="T5" s="8"/>
-      <c r="V5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="W5" s="8"/>
-      <c r="Y5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z5" s="8"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="14"/>
-      <c r="AE5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF5" s="8"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="14"/>
+      <c r="A5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="D5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="G5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="J5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="M5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="16"/>
+      <c r="P5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="16"/>
+      <c r="S5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="16"/>
+      <c r="V5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="W5" s="16"/>
+      <c r="Y5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="16"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="18"/>
+      <c r="AE5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF5" s="16"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="18"/>
     </row>
     <row r="8" spans="1:35" ht="8.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
@@ -931,51 +1042,51 @@
       <c r="AI11" s="1"/>
     </row>
     <row r="12" spans="1:35" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="2"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="J12" s="15" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="J12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N12" s="16"/>
+      <c r="N12" s="20"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="15" t="s">
+      <c r="P12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="16"/>
-      <c r="S12" s="15" t="s">
+      <c r="Q12" s="20"/>
+      <c r="S12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="T12" s="16"/>
+      <c r="T12" s="20"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="15" t="s">
+      <c r="V12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="W12" s="16"/>
+      <c r="W12" s="20"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="15" t="s">
+      <c r="Y12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="Z12" s="16"/>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="14"/>
+      <c r="Z12" s="20"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="18"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="15" t="s">
+      <c r="AE12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="AF12" s="16"/>
+      <c r="AF12" s="20"/>
       <c r="AG12" s="2"/>
-      <c r="AH12" s="13"/>
-      <c r="AI12" s="14"/>
+      <c r="AH12" s="17"/>
+      <c r="AI12" s="18"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="C13" s="1"/>
@@ -991,44 +1102,44 @@
       <c r="AI13" s="1"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="B14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="J14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="8"/>
-      <c r="M14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="P14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="8"/>
-      <c r="S14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="T14" s="8"/>
-      <c r="V14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="W14" s="8"/>
-      <c r="Y14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z14" s="8"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="14"/>
-      <c r="AE14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF14" s="8"/>
-      <c r="AH14" s="13"/>
-      <c r="AI14" s="14"/>
+      <c r="B14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="J14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="M14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="16"/>
+      <c r="P14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="16"/>
+      <c r="S14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="16"/>
+      <c r="V14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="W14" s="16"/>
+      <c r="Y14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="16"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="18"/>
+      <c r="AE14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="16"/>
+      <c r="AH14" s="17"/>
+      <c r="AI14" s="18"/>
     </row>
     <row r="17" spans="1:35" ht="8.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
@@ -1072,8 +1183,8 @@
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="K19" s="10" t="s">
         <v>5</v>
       </c>
@@ -1106,26 +1217,26 @@
       <c r="AF20" s="1"/>
     </row>
     <row r="21" spans="1:35" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="M21" s="15" t="s">
+      <c r="M21" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N21" s="16"/>
+      <c r="N21" s="20"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
-      <c r="V21" s="15" t="s">
+      <c r="V21" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="W21" s="16"/>
+      <c r="W21" s="20"/>
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
-      <c r="AE21" s="13"/>
-      <c r="AF21" s="14"/>
+      <c r="AE21" s="17"/>
+      <c r="AF21" s="18"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
     </row>
@@ -1136,79 +1247,43 @@
       <c r="AF22" s="1"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="D23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="M23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" s="8"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="V23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="W23" s="8"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="14"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
+      <c r="D23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="M23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="16"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="V23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="W23" s="16"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="25"/>
+      <c r="AE23" s="17"/>
+      <c r="AF23" s="18"/>
+      <c r="AG23" s="25"/>
+      <c r="AH23" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="T1:Y1"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K10:P10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AC10:AH10"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AH12:AI12"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AC19:AH19"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K19:P19"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
     <mergeCell ref="AB14:AC14"/>
     <mergeCell ref="AE14:AF14"/>
     <mergeCell ref="AH14:AI14"/>
@@ -1219,18 +1294,54 @@
     <mergeCell ref="S14:T14"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K19:P19"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AC19:AH19"/>
-    <mergeCell ref="AE21:AF21"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AC10:AH10"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AH12:AI12"/>
+    <mergeCell ref="K10:P10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1239,34 +1350,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB88519-6E38-4716-808F-E8354FD906F4}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="5">
         <v>45133</v>
       </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G11" s="23"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B5" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B6" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B10" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B13" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1276,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B69C7B3-E8BA-4B68-BD27-6FCF9A94D355}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F14"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1289,81 +1456,310 @@
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="285" x14ac:dyDescent="0.45">
       <c r="A1" s="6">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6">
+        <v>270</v>
+      </c>
+      <c r="E1" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="6">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6">
+        <v>100</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A3" s="6">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6">
+        <v>500</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="6">
+        <v>300</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="228" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="6">
+        <v>200</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="6">
+        <v>250</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A7" s="6">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6">
+        <v>150</v>
+      </c>
+      <c r="E7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A8" s="6">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="6">
+        <v>100</v>
+      </c>
+      <c r="E8" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="6">
+        <v>100</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A10" s="6">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="6">
+        <v>120</v>
+      </c>
+      <c r="E10" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A11" s="6">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="6">
+        <v>450</v>
+      </c>
+      <c r="E11" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A12" s="6">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="B12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6">
+        <v>370</v>
+      </c>
+      <c r="E12" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A13" s="6">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="6">
+      <c r="B13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="6">
+        <v>344</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A14" s="6">
+        <v>14</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="6">
+        <v>44</v>
+      </c>
+      <c r="E14" s="6">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A15" s="6">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="B15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="6">
+        <v>777</v>
+      </c>
+      <c r="E15" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="A16" s="6">
         <v>16</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="B16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="6">
+        <v>120</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A17" s="6">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="6">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="B17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="6">
+        <v>500</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="A18" s="6">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="6">
-        <v>58</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="6">
+      <c r="B18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="6">
+        <v>80</v>
+      </c>
+      <c r="E18" s="6">
         <v>1</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FrontEnn MenuCompleto Component funcionando perfectamente, falta actualizar algunas listas al editar
</commit_message>
<xml_diff>
--- a/control funciones menucompleto.xlsx
+++ b/control funciones menucompleto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jade_\Desktop\Delivery app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD6C97C-D1EA-4DEA-BA32-7E30DA06DB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50BAC07-8336-4E66-9413-E9744F5815DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{B50175D1-3EDE-4D77-9654-8E7F3090148C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t xml:space="preserve">AGREGAR TARJETA </t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>escritorio pattern</t>
+  </si>
+  <si>
+    <t>si se borrase un tipo de plato, y hubiese platos cargados, el id del plato borrado quedaria en la lista de platos con ese idTipoPlato borrado, entonces hay que resolver como arreglar esto</t>
   </si>
 </sst>
 </file>
@@ -371,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -386,66 +389,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,58 +826,58 @@
       <c r="AI2" s="1"/>
     </row>
     <row r="3" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="J3" s="24" t="s">
+      <c r="H3" s="17"/>
+      <c r="J3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="25"/>
+      <c r="K3" s="17"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="25"/>
+      <c r="N3" s="17"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="S3" s="24" t="s">
+      <c r="Q3" s="17"/>
+      <c r="S3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="25"/>
+      <c r="T3" s="17"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="24" t="s">
+      <c r="V3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="25"/>
+      <c r="W3" s="17"/>
       <c r="X3" s="2"/>
-      <c r="Y3" s="24" t="s">
+      <c r="Y3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="25"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="21"/>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="24" t="s">
+      <c r="AE3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AF3" s="25"/>
+      <c r="AF3" s="17"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="16"/>
-      <c r="AI3" s="17"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="21"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
@@ -895,50 +894,50 @@
       <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="D5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="G5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="J5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="11"/>
-      <c r="M5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="11"/>
-      <c r="P5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="11"/>
-      <c r="S5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="T5" s="11"/>
-      <c r="V5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="W5" s="11"/>
-      <c r="Y5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z5" s="11"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="17"/>
-      <c r="AE5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF5" s="11"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="17"/>
+      <c r="A5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="J5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="M5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="19"/>
+      <c r="P5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="19"/>
+      <c r="S5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="19"/>
+      <c r="V5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="W5" s="19"/>
+      <c r="Y5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="19"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="21"/>
+      <c r="AE5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF5" s="19"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="21"/>
     </row>
     <row r="8" spans="1:35" ht="8.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
@@ -1023,51 +1022,51 @@
       <c r="AI11" s="1"/>
     </row>
     <row r="12" spans="1:35" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="2"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="J12" s="18" t="s">
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+      <c r="J12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="19"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="18" t="s">
+      <c r="M12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="N12" s="19"/>
+      <c r="N12" s="23"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="18" t="s">
+      <c r="P12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="19"/>
-      <c r="S12" s="18" t="s">
+      <c r="Q12" s="23"/>
+      <c r="S12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="T12" s="19"/>
+      <c r="T12" s="23"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="18" t="s">
+      <c r="V12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="W12" s="19"/>
+      <c r="W12" s="23"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="18" t="s">
+      <c r="Y12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="Z12" s="19"/>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="17"/>
+      <c r="Z12" s="23"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="21"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="18" t="s">
+      <c r="AE12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="AF12" s="19"/>
+      <c r="AF12" s="23"/>
       <c r="AG12" s="2"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="17"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="21"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="C13" s="1"/>
@@ -1083,44 +1082,44 @@
       <c r="AI13" s="1"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="B14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="J14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="11"/>
-      <c r="M14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="11"/>
-      <c r="P14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="11"/>
-      <c r="S14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="T14" s="11"/>
-      <c r="V14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="W14" s="11"/>
-      <c r="Y14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z14" s="11"/>
-      <c r="AB14" s="16"/>
-      <c r="AC14" s="17"/>
-      <c r="AE14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF14" s="11"/>
-      <c r="AH14" s="16"/>
-      <c r="AI14" s="17"/>
+      <c r="B14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="J14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="M14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="19"/>
+      <c r="P14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="19"/>
+      <c r="S14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="19"/>
+      <c r="V14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="W14" s="19"/>
+      <c r="Y14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="19"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="21"/>
+      <c r="AE14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="19"/>
+      <c r="AH14" s="20"/>
+      <c r="AI14" s="21"/>
     </row>
     <row r="17" spans="1:35" ht="8.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
@@ -1164,8 +1163,8 @@
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
       <c r="K19" s="13" t="s">
         <v>5</v>
       </c>
@@ -1198,26 +1197,26 @@
       <c r="AF20" s="1"/>
     </row>
     <row r="21" spans="1:35" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="19"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="M21" s="18" t="s">
+      <c r="M21" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="N21" s="19"/>
+      <c r="N21" s="23"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
-      <c r="V21" s="18" t="s">
+      <c r="V21" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="W21" s="19"/>
+      <c r="W21" s="23"/>
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
-      <c r="AE21" s="16"/>
-      <c r="AF21" s="17"/>
+      <c r="AE21" s="20"/>
+      <c r="AF21" s="21"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
     </row>
@@ -1228,79 +1227,43 @@
       <c r="AF22" s="1"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="D23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="M23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" s="11"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="V23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="W23" s="11"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="AE23" s="16"/>
-      <c r="AF23" s="17"/>
-      <c r="AG23" s="12"/>
-      <c r="AH23" s="12"/>
+      <c r="D23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="M23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="19"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="V23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="W23" s="19"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="28"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="21"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="T1:Y1"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K10:P10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AC10:AH10"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AH12:AI12"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AC19:AH19"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K19:P19"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
     <mergeCell ref="AB14:AC14"/>
     <mergeCell ref="AE14:AF14"/>
     <mergeCell ref="AH14:AI14"/>
@@ -1311,18 +1274,54 @@
     <mergeCell ref="S14:T14"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K19:P19"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AC19:AH19"/>
-    <mergeCell ref="AE21:AF21"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AC10:AH10"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AH12:AI12"/>
+    <mergeCell ref="K10:P10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1331,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB88519-6E38-4716-808F-E8354FD906F4}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1401,7 +1400,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1414,6 +1413,11 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B14" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1437,16 +1441,16 @@
     <col min="3" max="3" width="39.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="26"/>
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="10"/>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="6"/>
@@ -1483,10 +1487,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="6"/>
@@ -1495,7 +1499,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="28"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
@@ -1544,7 +1548,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="28"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>

</xml_diff>